<commit_message>
Finished speed telemetry sending, converted to km/h
</commit_message>
<xml_diff>
--- a/sensor-module/speed_unitscale.xlsx
+++ b/sensor-module/speed_unitscale.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TSEA29\projekt\sensor-module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43B357FD-C749-4888-8B10-ED3C8C75DE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC27E45-0C31-43DF-9BD6-0DE2440CAC4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{2130E81C-8F6F-43E1-8E36-7F0E930A4D1A}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890" xr2:uid="{2130E81C-8F6F-43E1-8E36-7F0E930A4D1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Km/h</t>
   </si>
@@ -62,19 +53,36 @@
   <si>
     <t>km/h från 5ticks, decimaljusterat</t>
   </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> us</t>
+  </si>
+  <si>
+    <t>duty cycle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="176" formatCode="0.0000000"/>
-    <numFmt numFmtId="178" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000"/>
+    <numFmt numFmtId="172" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,20 +108,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -126,13 +137,13 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="166" formatCode="0.00000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.00000"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -150,18 +161,18 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1824E309-61C3-4CCC-95F1-9C1835FDB95F}" name="Tabell1" displayName="Tabell1" ref="A1:F44" totalsRowShown="0">
   <autoFilter ref="A1:F44" xr:uid="{1824E309-61C3-4CCC-95F1-9C1835FDB95F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E44">
+  <sortState ref="A2:E44">
     <sortCondition ref="A1:A44"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AC889DC7-85AB-4F31-A343-EE49B0A217E4}" name="Km/h" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{E362EA7C-050D-4B5C-9C4E-D6286D5E1F74}" name="m/s" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{AC889DC7-85AB-4F31-A343-EE49B0A217E4}" name="Km/h" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{E362EA7C-050D-4B5C-9C4E-D6286D5E1F74}" name="m/s" dataDxfId="4">
       <calculatedColumnFormula>A2*(1000/3600)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4E1ED850-2647-48D7-98CB-163286C7D01B}" name="m/ms" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{4E1ED850-2647-48D7-98CB-163286C7D01B}" name="m/ms" dataDxfId="3">
       <calculatedColumnFormula>Tabell1[[#This Row],[m/s]]/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A91EA2FE-8186-4485-86B5-3DE7BADBBD9D}" name="ticks/s" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{A91EA2FE-8186-4485-86B5-3DE7BADBBD9D}" name="ticks/s" dataDxfId="2">
       <calculatedColumnFormula>Tabell1[[#This Row],[m/s]]/0.13*5</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{D79CF248-49CB-4799-B4AA-064CB94B298F}" name="Δtick (ms)" dataDxfId="1">
@@ -176,7 +187,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -472,23 +483,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5DEB989-7240-4E26-B4F0-A6281BB06622}">
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,12 +534,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0.25</v>
       </c>
       <c r="B2" s="2">
-        <f>A2*(1000/3600)</f>
+        <f t="shared" ref="B2:B44" si="0">A2*(1000/3600)</f>
         <v>6.9444444444444448E-2</v>
       </c>
       <c r="C2" s="4">
@@ -572,12 +583,12 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
       <c r="B3" s="2">
-        <f>A3*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>0.1388888888888889</v>
       </c>
       <c r="C3" s="4">
@@ -614,12 +625,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.75</v>
       </c>
       <c r="B4" s="2">
-        <f>A4*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>0.20833333333333334</v>
       </c>
       <c r="C4" s="4">
@@ -651,12 +662,12 @@
         <v>0.24999999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>0.9</v>
       </c>
       <c r="B5" s="2">
-        <f>A5*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="C5" s="4">
@@ -684,12 +695,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6" s="2">
-        <f>A6*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="C6" s="4">
@@ -717,12 +728,12 @@
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1.8</v>
       </c>
       <c r="B7" s="2">
-        <f>A7*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="C7" s="4">
@@ -750,12 +761,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2</v>
       </c>
       <c r="B8" s="2">
-        <f>A8*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="C8" s="4">
@@ -783,12 +794,12 @@
         <v>199.99999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2.7</v>
       </c>
       <c r="B9" s="2">
-        <f>A9*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>0.75000000000000011</v>
       </c>
       <c r="C9" s="4">
@@ -816,12 +827,12 @@
         <v>270.00000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>3</v>
       </c>
       <c r="B10" s="2">
-        <f>A10*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="C10" s="4">
@@ -849,12 +860,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3.6</v>
       </c>
       <c r="B11" s="2">
-        <f>A11*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C11" s="4">
@@ -882,12 +893,12 @@
         <v>360</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>4</v>
       </c>
       <c r="B12" s="2">
-        <f>A12*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>1.1111111111111112</v>
       </c>
       <c r="C12" s="4">
@@ -915,12 +926,12 @@
         <v>399.99999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>4.5</v>
       </c>
       <c r="B13" s="2">
-        <f>A13*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
       <c r="C13" s="4">
@@ -948,12 +959,12 @@
         <v>450</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>5</v>
       </c>
       <c r="B14" s="2">
-        <f>A14*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>1.3888888888888888</v>
       </c>
       <c r="C14" s="4">
@@ -981,12 +992,12 @@
         <v>499.99999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>5.4</v>
       </c>
       <c r="B15" s="2">
-        <f>A15*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>1.5000000000000002</v>
       </c>
       <c r="C15" s="4">
@@ -1014,12 +1025,12 @@
         <v>540.00000000000011</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>6</v>
       </c>
       <c r="B16" s="2">
-        <f>A16*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="C16" s="4">
@@ -1047,12 +1058,12 @@
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>6.3</v>
       </c>
       <c r="B17" s="2">
-        <f>A17*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
       <c r="C17" s="4">
@@ -1080,12 +1091,12 @@
         <v>630</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>7</v>
       </c>
       <c r="B18" s="2">
-        <f>A18*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>1.9444444444444446</v>
       </c>
       <c r="C18" s="4">
@@ -1113,12 +1124,12 @@
         <v>700</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>7.2</v>
       </c>
       <c r="B19" s="2">
-        <f>A19*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C19" s="4">
@@ -1146,12 +1157,12 @@
         <v>720</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>8</v>
       </c>
       <c r="B20" s="2">
-        <f>A20*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>2.2222222222222223</v>
       </c>
       <c r="C20" s="4">
@@ -1179,12 +1190,12 @@
         <v>799.99999999999989</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>9</v>
       </c>
       <c r="B21" s="2">
-        <f>A21*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="C21" s="4">
@@ -1212,12 +1223,12 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>9</v>
       </c>
       <c r="B22" s="2">
-        <f>A22*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="C22" s="4">
@@ -1245,12 +1256,12 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>10</v>
       </c>
       <c r="B23" s="2">
-        <f>A23*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>2.7777777777777777</v>
       </c>
       <c r="C23" s="4">
@@ -1278,12 +1289,12 @@
         <v>999.99999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>10.8</v>
       </c>
       <c r="B24" s="2">
-        <f>A24*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>3.0000000000000004</v>
       </c>
       <c r="C24" s="4">
@@ -1311,12 +1322,12 @@
         <v>1080.0000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>12.5</v>
       </c>
       <c r="B25" s="2">
-        <f>A25*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>3.4722222222222223</v>
       </c>
       <c r="C25" s="4">
@@ -1344,12 +1355,12 @@
         <v>1249.9999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>12.6</v>
       </c>
       <c r="B26" s="2">
-        <f>A26*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="C26" s="4">
@@ -1377,12 +1388,12 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>14.4</v>
       </c>
       <c r="B27" s="2">
-        <f>A27*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C27" s="4">
@@ -1410,12 +1421,12 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>15</v>
       </c>
       <c r="B28" s="2">
-        <f>A28*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>4.166666666666667</v>
       </c>
       <c r="C28" s="4">
@@ -1442,13 +1453,22 @@
         <f>46800/Tabell1[[#This Row],[Δ5ticks (ms)]]</f>
         <v>1499.9999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="S28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T28" t="s">
+        <v>10</v>
+      </c>
+      <c r="V28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>16.2</v>
       </c>
       <c r="B29" s="2">
-        <f>A29*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="C29" s="4">
@@ -1475,13 +1495,24 @@
         <f>46800/Tabell1[[#This Row],[Δ5ticks (ms)]]</f>
         <v>1619.9999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="S29">
+        <v>60</v>
+      </c>
+      <c r="T29">
+        <f>S29*1000</f>
+        <v>60000</v>
+      </c>
+      <c r="V29" s="7">
+        <f>T30/T29</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>17.5</v>
       </c>
       <c r="B30" s="2">
-        <f>A30*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>4.8611111111111116</v>
       </c>
       <c r="C30" s="4">
@@ -1508,13 +1539,20 @@
         <f>46800/Tabell1[[#This Row],[Δ5ticks (ms)]]</f>
         <v>1750.0000000000007</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="S30">
+        <f>T30/1000</f>
+        <v>0.01</v>
+      </c>
+      <c r="T30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>18</v>
       </c>
       <c r="B31" s="2">
-        <f>A31*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C31" s="4">
@@ -1542,12 +1580,12 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>20</v>
       </c>
       <c r="B32" s="2">
-        <f>A32*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>5.5555555555555554</v>
       </c>
       <c r="C32" s="4">
@@ -1575,12 +1613,12 @@
         <v>1999.9999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>21.6</v>
       </c>
       <c r="B33" s="2">
-        <f>A33*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>6.0000000000000009</v>
       </c>
       <c r="C33" s="4">
@@ -1608,12 +1646,12 @@
         <v>2160.0000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>22.5</v>
       </c>
       <c r="B34" s="2">
-        <f>A34*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
       <c r="C34" s="4">
@@ -1641,12 +1679,12 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>25</v>
       </c>
       <c r="B35" s="2">
-        <f>A35*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>6.9444444444444446</v>
       </c>
       <c r="C35" s="4">
@@ -1674,12 +1712,12 @@
         <v>2499.9999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>25.2</v>
       </c>
       <c r="B36" s="2">
-        <f>A36*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C36" s="4">
@@ -1707,12 +1745,12 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>27.5</v>
       </c>
       <c r="B37" s="2">
-        <f>A37*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>7.6388888888888893</v>
       </c>
       <c r="C37" s="4">
@@ -1740,12 +1778,12 @@
         <v>2750.0000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>28.8</v>
       </c>
       <c r="B38" s="2">
-        <f>A38*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C38" s="4">
@@ -1773,12 +1811,12 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>30</v>
       </c>
       <c r="B39" s="2">
-        <f>A39*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="C39" s="4">
@@ -1806,12 +1844,12 @@
         <v>2999.9999999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>32.4</v>
       </c>
       <c r="B40" s="2">
-        <f>A40*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C40" s="4">
@@ -1839,12 +1877,12 @@
         <v>3239.9999999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>35</v>
       </c>
       <c r="B41" s="2">
-        <f>A41*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>9.7222222222222232</v>
       </c>
       <c r="C41" s="4">
@@ -1872,12 +1910,12 @@
         <v>3500.0000000000014</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>36</v>
       </c>
       <c r="B42" s="2">
-        <f>A42*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C42" s="4">
@@ -1905,12 +1943,12 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>36</v>
       </c>
       <c r="B43" s="2">
-        <f>A43*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C43" s="4">
@@ -1938,12 +1976,12 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>40</v>
       </c>
       <c r="B44" s="2">
-        <f>A44*(1000/3600)</f>
+        <f t="shared" si="0"/>
         <v>11.111111111111111</v>
       </c>
       <c r="C44" s="4">
@@ -1973,8 +2011,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>